<commit_message>
Update R script paths for PBA40 -> RTP plus IPA model run names
</commit_message>
<xml_diff>
--- a/utilities/RTP/Emissions/ModelRuns.xlsx
+++ b/utilities/RTP/Emissions/ModelRuns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\PBA40\Emissions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\Emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F3771E-7138-4A2E-B95B-CD9F6DAF4E73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B648F0-4597-4359-9F9E-0C0C7D1BB906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12045" yWindow="2715" windowWidth="14430" windowHeight="10575" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16920" yWindow="720" windowWidth="18900" windowHeight="11805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTP2017" sheetId="1" r:id="rId1"/>
@@ -109,28 +109,28 @@
     <t>2035_06_694_Amd1</t>
   </si>
   <si>
-    <t>2035_TM151_IPA_loPop_loAOC_00</t>
-  </si>
-  <si>
     <t>IP</t>
   </si>
   <si>
-    <t>2035_TM151_IPA_loPop_hiAOC_00</t>
-  </si>
-  <si>
-    <t>2035_TM151_IPA_hiPop_loAOC_00</t>
-  </si>
-  <si>
-    <t>2035_TM151_IPA_hiPop_hiAOC_00</t>
-  </si>
-  <si>
-    <t>IP_hiAOC</t>
-  </si>
-  <si>
-    <t>IP_hiPop</t>
-  </si>
-  <si>
-    <t>IP_hiPop_hiAOC</t>
+    <t>2005_TM152_IPA_02</t>
+  </si>
+  <si>
+    <t>2035_TM152_IPA_aoc1421_00</t>
+  </si>
+  <si>
+    <t>2035_TM152_IPA_aoc1562_00</t>
+  </si>
+  <si>
+    <t>2035_TM152_IPA_aoc1795_00</t>
+  </si>
+  <si>
+    <t>IP_aoc1421</t>
+  </si>
+  <si>
+    <t>IP_aoc1562</t>
+  </si>
+  <si>
+    <t>IP_aoc1795</t>
   </si>
 </sst>
 </file>
@@ -704,7 +704,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,13 +727,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>2035</v>
+        <v>2005</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update paths for RTP2021 IP runs
</commit_message>
<xml_diff>
--- a/utilities/RTP/Emissions/ModelRuns.xlsx
+++ b/utilities/RTP/Emissions/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\Emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B648F0-4597-4359-9F9E-0C0C7D1BB906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A037882-B936-4875-B6AE-08F289AB39D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="720" windowWidth="18900" windowHeight="11805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10170" yWindow="1515" windowWidth="27990" windowHeight="18750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTP2017" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>2005_05_003</t>
   </si>
@@ -112,25 +112,13 @@
     <t>IP</t>
   </si>
   <si>
-    <t>2005_TM152_IPA_02</t>
-  </si>
-  <si>
-    <t>2035_TM152_IPA_aoc1421_00</t>
-  </si>
-  <si>
-    <t>2035_TM152_IPA_aoc1562_00</t>
-  </si>
-  <si>
-    <t>2035_TM152_IPA_aoc1795_00</t>
-  </si>
-  <si>
-    <t>IP_aoc1421</t>
-  </si>
-  <si>
-    <t>IP_aoc1562</t>
-  </si>
-  <si>
-    <t>IP_aoc1795</t>
+    <t>2005_TM152_IPA_03</t>
+  </si>
+  <si>
+    <t>2015_TM152_IPA_16</t>
+  </si>
+  <si>
+    <t>2035_TM152_IPA_00</t>
   </si>
 </sst>
 </file>
@@ -700,11 +688,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170D2EFC-85A6-4F44-9439-D7E63C3E4D90}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,13 +726,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2035</v>
+        <v>2015</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,18 +743,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>2035</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added draft blueprint run set to Emissions calculator
And updated BikeInfrastructure.R for paths
</commit_message>
<xml_diff>
--- a/utilities/RTP/Emissions/ModelRuns.xlsx
+++ b/utilities/RTP/Emissions/ModelRuns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\RTP\Emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A037882-B936-4875-B6AE-08F289AB39D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97A13DB-7B80-4BA5-B1D0-7A26A1B6AD80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10170" yWindow="1515" windowWidth="27990" windowHeight="18750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16680" yWindow="6465" windowWidth="15510" windowHeight="13080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTP2017" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>2005_05_003</t>
   </si>
@@ -119,6 +119,33 @@
   </si>
   <si>
     <t>2035_TM152_IPA_00</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_PlusCrossing_01</t>
+  </si>
+  <si>
+    <t>Plus Crossing</t>
+  </si>
+  <si>
+    <t>run_set</t>
+  </si>
+  <si>
+    <t>2050_TM152_DBP_Basic_00</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_Basic_00</t>
+  </si>
+  <si>
+    <t>2035_TM152_DBP_Plus_01</t>
+  </si>
+  <si>
+    <t>Plus</t>
+  </si>
+  <si>
+    <t>DraftBlueprint</t>
   </si>
 </sst>
 </file>
@@ -688,21 +715,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170D2EFC-85A6-4F44-9439-D7E63C3E4D90}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -710,10 +738,13 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2005</v>
       </c>
@@ -723,8 +754,11 @@
       <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2015</v>
       </c>
@@ -734,8 +768,11 @@
       <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2035</v>
       </c>
@@ -744,6 +781,65 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2050</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2050</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>